<commit_message>
email not send none
</commit_message>
<xml_diff>
--- a/small.xlsx
+++ b/small.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>ردیف</t>
   </si>
@@ -112,9 +112,6 @@
     <t>مهرداد مریدی نژاد</t>
   </si>
   <si>
-    <t>mehrdad.moridinejad@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">احمد علیپور </t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>رضا افشاری فر</t>
-  </si>
-  <si>
-    <t>testmail3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -140,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -176,6 +170,7 @@
     <font>
       <b/>
       <sz val="14.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -185,20 +180,12 @@
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="18.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -332,7 +319,7 @@
     <xf borderId="3" fillId="0" fontId="8" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="2" fontId="7" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="4" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -354,21 +341,21 @@
     <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -384,10 +371,10 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -830,16 +817,16 @@
         <v>31</v>
       </c>
       <c r="AF3" s="30"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="31"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="31"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="30"/>
+      <c r="AJ3" s="30"/>
     </row>
     <row r="4">
       <c r="A4" s="14">
         <v>2.0</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="16">
@@ -912,24 +899,22 @@
         <f t="shared" si="9"/>
         <v>23400000</v>
       </c>
-      <c r="AD4" s="33" t="s">
+      <c r="AD4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AE4" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="31"/>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="31"/>
-      <c r="AJ4" s="31"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="30"/>
     </row>
     <row r="5">
       <c r="A5" s="14">
         <v>3.0</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="16">
         <v>30.0</v>
@@ -1002,23 +987,23 @@
         <v>28000000</v>
       </c>
       <c r="AD5" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="AE5" s="29" t="s">
-        <v>35</v>
-      </c>
       <c r="AF5" s="30"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="31"/>
-      <c r="AI5" s="31"/>
-      <c r="AJ5" s="31"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="30"/>
     </row>
     <row r="6">
       <c r="A6" s="14">
         <v>4.0</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="16">
         <v>30.0</v>
@@ -1089,23 +1074,23 @@
         <v>23000000</v>
       </c>
       <c r="AD6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AE6" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF6" s="31"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="31"/>
-      <c r="AI6" s="31"/>
-      <c r="AJ6" s="31"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
     </row>
     <row r="7">
       <c r="A7" s="14">
         <v>5.0</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="16">
         <v>30.0</v>
@@ -1180,16 +1165,14 @@
         <v>39861027.8</v>
       </c>
       <c r="AD7" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="31"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="31"/>
+        <v>37</v>
+      </c>
+      <c r="AE7" s="33"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>